<commit_message>
corrigindo modelo de relatorio em excel
</commit_message>
<xml_diff>
--- a/backend/src/utils/modelo relatiorio excel.xlsx
+++ b/backend/src/utils/modelo relatiorio excel.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">CST</t>
   </si>
   <si>
-    <t xml:space="preserve">cClasTrib</t>
+    <t xml:space="preserve">cClassTrib</t>
   </si>
   <si>
     <t xml:space="preserve">Aliquota IBS</t>
@@ -144,20 +144,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,13 +256,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Figura 1" descr=""/>
+        <xdr:cNvPr id="1" name="Picture 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -258,9 +270,9 @@
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="4800">
-          <a:off x="720" y="1080"/>
-          <a:ext cx="1785240" cy="1171800"/>
+        <a:xfrm>
+          <a:off x="1080" y="1440"/>
+          <a:ext cx="1784880" cy="1165320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -453,70 +465,98 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="B2:F3"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>